<commit_message>
Features added - Execution on Safari Browser, ExtentReport name
</commit_message>
<xml_diff>
--- a/Test_Execution_Reports_Analysis/Test_Suite_Execution_Report_Analysis.xlsx
+++ b/Test_Execution_Reports_Analysis/Test_Suite_Execution_Report_Analysis.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nagarro-my.sharepoint.com/personal/rajat_verma01_nagarro_com/Documents/GIT_Projects/New folder/Test_Execution_Reports_Analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work_In_Local_Machine\Eclipse_Java_Developers_06_2021\LearningWS\Final_Code\52_Framework_Selenium_TestNG_Final_Parallel\extent_reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{4A4C7B1B-1D4A-478D-8BF9-7900D68C616C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5DF88BA4-0493-40B4-B97B-AA8B11A7D119}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851DCDFC-510C-441B-B9F7-74652E6EC527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Test_Execution" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -59,40 +59,48 @@
     <t>2 min 14 sec</t>
   </si>
   <si>
-    <t>2 min 21 sec</t>
-  </si>
-  <si>
-    <t>01_TestNG_Execute_Sequential_Regression</t>
-  </si>
-  <si>
-    <t>2 min 38 sec</t>
-  </si>
-  <si>
-    <t>02_TestNG_Execute_Parallel_Regression</t>
-  </si>
-  <si>
-    <t>03_TestNG_Execute_Parallel_MB_Regression</t>
-  </si>
-  <si>
-    <t>2 min 28 sec</t>
-  </si>
-  <si>
-    <t>1 min 3 sec</t>
-  </si>
-  <si>
-    <t>1 min 0 sec</t>
-  </si>
-  <si>
-    <t>0 min 54 sec</t>
+    <t>2 min 48 sec</t>
+  </si>
+  <si>
+    <t>2 min 18 sec</t>
+  </si>
+  <si>
+    <t>2 min 33 sec</t>
+  </si>
+  <si>
+    <t>1 min 14 sec</t>
+  </si>
+  <si>
+    <t>0 min 56 sec</t>
+  </si>
+  <si>
+    <t>1 min 4 sec</t>
+  </si>
+  <si>
+    <t>1 min 18 sec</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>WINDOWS 10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -107,15 +115,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -258,73 +272,31 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -605,105 +577,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:J9"/>
+  <dimension ref="C5:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:I9"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="38.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.90625" customWidth="1"/>
+    <col min="3" max="3" width="24.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="10" t="s">
+    <row r="5" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="6" spans="3:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="C7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="G7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="4"/>
+      <c r="J7" s="5"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B3" s="11" t="s">
+    <row r="8" spans="3:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="12" t="s">
+      <c r="F8" s="7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="D6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="D7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="1" t="s">
+      <c r="G8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="6"/>
-    </row>
-    <row r="8" spans="2:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="D8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="H8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="6"/>
-    </row>
-    <row r="9" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D9" s="7"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="9"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>